<commit_message>
adds mill and deer 2022 efficiency data
</commit_message>
<xml_diff>
--- a/data-raw/metadata/deer_mill_recapture_metadata.xlsx
+++ b/data-raw/metadata/deer_mill_recapture_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-deer-mill-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincain/Documents/Git/JPE/jpe-deer-mill-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ECB94F-05CD-6E4E-93D7-89B41BBE39EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C119C71C-99BE-9040-BF84-FB90576569CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="760" windowWidth="27680" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="800" windowWidth="27680" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -73,16 +73,10 @@
     <t>text</t>
   </si>
   <si>
-    <t>Fork length of the fish measured in millimeters</t>
-  </si>
-  <si>
     <t>ratio</t>
   </si>
   <si>
     <t>numeric</t>
-  </si>
-  <si>
-    <t>real</t>
   </si>
   <si>
     <t>dateTime</t>
@@ -97,28 +91,61 @@
     <t>attribute_name</t>
   </si>
   <si>
-    <t>millimeter</t>
-  </si>
-  <si>
     <t>recapture</t>
   </si>
   <si>
-    <t>date</t>
+    <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
   <si>
-    <t>fork_length</t>
+    <t>release_id</t>
   </si>
   <si>
-    <t>lifestage</t>
+    <t xml:space="preserve">Unique identifier assigned to each release trial ( stream name, year, release trial ) </t>
   </si>
   <si>
-    <t>Life stage of the fish. Levels = c("silvery parr", "smolt", "parr", "fry", "sac fry")</t>
+    <t>release</t>
   </si>
   <si>
-    <t>Date and time of day associated with the trap visit</t>
+    <t>stream</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
+    <t>Name of stream where fish released</t>
+  </si>
+  <si>
+    <t>Date and time of recaptures</t>
+  </si>
+  <si>
+    <t>number of fish</t>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean fork length of recaptured fish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min fork length of recaptured fish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max fork length of recaptured fish </t>
+  </si>
+  <si>
+    <t>total_recaptured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of fish recaptured associated with a given release trial </t>
+  </si>
+  <si>
+    <t>recapture_date</t>
+  </si>
+  <si>
+    <t>mean_fl_recaptured</t>
+  </si>
+  <si>
+    <t>min_fl_recaptured</t>
+  </si>
+  <si>
+    <t>max_fl_recaptured</t>
   </si>
 </sst>
 </file>
@@ -426,11 +453,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z967"/>
+  <dimension ref="A1:Z972"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -505,35 +532,29 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="9">
-        <v>44601</v>
-      </c>
-      <c r="M2" s="8">
-        <v>44657</v>
-      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -553,35 +574,25 @@
         <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="3">
-        <v>43</v>
-      </c>
-      <c r="M3" s="3">
-        <v>77</v>
-      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -597,29 +608,35 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>27</v>
+      <c r="A4" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
+      <c r="L4" s="9">
+        <v>44601</v>
+      </c>
+      <c r="M4" s="8">
+        <v>44657</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -634,20 +651,40 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+    <row r="5" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="L5" s="3">
+        <v>10</v>
+      </c>
+      <c r="M5" s="3">
+        <v>100</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -662,20 +699,40 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+    <row r="6" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="L6" s="3">
+        <v>10</v>
+      </c>
+      <c r="M6" s="3">
+        <v>100</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -690,19 +747,40 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+    <row r="7" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="L7" s="3">
+        <v>10</v>
+      </c>
+      <c r="M7" s="3">
+        <v>100</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -717,20 +795,40 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+    <row r="8" spans="1:26" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>400</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -830,7 +928,6 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
@@ -1670,7 +1767,7 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
@@ -1698,7 +1795,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
+      <c r="A43" s="4"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
@@ -1726,7 +1823,7 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
+      <c r="A44" s="4"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
@@ -1754,7 +1851,7 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
@@ -1782,7 +1879,7 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
+      <c r="A46" s="4"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
@@ -27597,18 +27694,158 @@
       <c r="Y967" s="1"/>
       <c r="Z967" s="1"/>
     </row>
+    <row r="968" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A968" s="1"/>
+      <c r="B968" s="1"/>
+      <c r="C968" s="1"/>
+      <c r="D968" s="2"/>
+      <c r="E968" s="1"/>
+      <c r="F968" s="3"/>
+      <c r="G968" s="3"/>
+      <c r="H968" s="3"/>
+      <c r="I968" s="2"/>
+      <c r="J968" s="3"/>
+      <c r="K968" s="2"/>
+      <c r="L968" s="3"/>
+      <c r="M968" s="3"/>
+      <c r="N968" s="1"/>
+      <c r="O968" s="1"/>
+      <c r="P968" s="1"/>
+      <c r="Q968" s="1"/>
+      <c r="R968" s="1"/>
+      <c r="S968" s="1"/>
+      <c r="T968" s="1"/>
+      <c r="U968" s="1"/>
+      <c r="V968" s="1"/>
+      <c r="W968" s="1"/>
+      <c r="X968" s="1"/>
+      <c r="Y968" s="1"/>
+      <c r="Z968" s="1"/>
+    </row>
+    <row r="969" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A969" s="1"/>
+      <c r="B969" s="1"/>
+      <c r="C969" s="1"/>
+      <c r="D969" s="2"/>
+      <c r="E969" s="1"/>
+      <c r="F969" s="3"/>
+      <c r="G969" s="3"/>
+      <c r="H969" s="3"/>
+      <c r="I969" s="2"/>
+      <c r="J969" s="3"/>
+      <c r="K969" s="2"/>
+      <c r="L969" s="3"/>
+      <c r="M969" s="3"/>
+      <c r="N969" s="1"/>
+      <c r="O969" s="1"/>
+      <c r="P969" s="1"/>
+      <c r="Q969" s="1"/>
+      <c r="R969" s="1"/>
+      <c r="S969" s="1"/>
+      <c r="T969" s="1"/>
+      <c r="U969" s="1"/>
+      <c r="V969" s="1"/>
+      <c r="W969" s="1"/>
+      <c r="X969" s="1"/>
+      <c r="Y969" s="1"/>
+      <c r="Z969" s="1"/>
+    </row>
+    <row r="970" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A970" s="1"/>
+      <c r="B970" s="1"/>
+      <c r="C970" s="1"/>
+      <c r="D970" s="2"/>
+      <c r="E970" s="1"/>
+      <c r="F970" s="3"/>
+      <c r="G970" s="3"/>
+      <c r="H970" s="3"/>
+      <c r="I970" s="2"/>
+      <c r="J970" s="3"/>
+      <c r="K970" s="2"/>
+      <c r="L970" s="3"/>
+      <c r="M970" s="3"/>
+      <c r="N970" s="1"/>
+      <c r="O970" s="1"/>
+      <c r="P970" s="1"/>
+      <c r="Q970" s="1"/>
+      <c r="R970" s="1"/>
+      <c r="S970" s="1"/>
+      <c r="T970" s="1"/>
+      <c r="U970" s="1"/>
+      <c r="V970" s="1"/>
+      <c r="W970" s="1"/>
+      <c r="X970" s="1"/>
+      <c r="Y970" s="1"/>
+      <c r="Z970" s="1"/>
+    </row>
+    <row r="971" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A971" s="1"/>
+      <c r="B971" s="1"/>
+      <c r="C971" s="1"/>
+      <c r="D971" s="2"/>
+      <c r="E971" s="1"/>
+      <c r="F971" s="3"/>
+      <c r="G971" s="3"/>
+      <c r="H971" s="3"/>
+      <c r="I971" s="2"/>
+      <c r="J971" s="3"/>
+      <c r="K971" s="2"/>
+      <c r="L971" s="3"/>
+      <c r="M971" s="3"/>
+      <c r="N971" s="1"/>
+      <c r="O971" s="1"/>
+      <c r="P971" s="1"/>
+      <c r="Q971" s="1"/>
+      <c r="R971" s="1"/>
+      <c r="S971" s="1"/>
+      <c r="T971" s="1"/>
+      <c r="U971" s="1"/>
+      <c r="V971" s="1"/>
+      <c r="W971" s="1"/>
+      <c r="X971" s="1"/>
+      <c r="Y971" s="1"/>
+      <c r="Z971" s="1"/>
+    </row>
+    <row r="972" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A972" s="1"/>
+      <c r="B972" s="1"/>
+      <c r="C972" s="1"/>
+      <c r="D972" s="2"/>
+      <c r="E972" s="1"/>
+      <c r="F972" s="3"/>
+      <c r="G972" s="3"/>
+      <c r="H972" s="3"/>
+      <c r="I972" s="2"/>
+      <c r="J972" s="3"/>
+      <c r="K972" s="2"/>
+      <c r="L972" s="3"/>
+      <c r="M972" s="3"/>
+      <c r="N972" s="1"/>
+      <c r="O972" s="1"/>
+      <c r="P972" s="1"/>
+      <c r="Q972" s="1"/>
+      <c r="R972" s="1"/>
+      <c r="S972" s="1"/>
+      <c r="T972" s="1"/>
+      <c r="U972" s="1"/>
+      <c r="V972" s="1"/>
+      <c r="W972" s="1"/>
+      <c r="X972" s="1"/>
+      <c r="Y972" s="1"/>
+      <c r="Z972" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C24:C967 C1:C12 E2" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C29:C972 E4 C1:C17" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1 E3:E967 G2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E3 G4 E5:E972" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1 F3:F967 H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F3 H4 F5:F972" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1 H3:H967" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H3 H5:H972" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27635,13 +27872,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>

</xml_diff>